<commit_message>
commit before modifying fixed pt to work with signed
</commit_message>
<xml_diff>
--- a/scripts/codegen/CAN/CanMsgs.xlsx
+++ b/scripts/codegen/CAN/CanMsgs.xlsx
@@ -2072,10 +2072,10 @@
   <dimension ref="A1:AE1039"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="H347" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="K51" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="G365" sqref="G365"/>
+      <selection pane="bottomRight" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>